<commit_message>
add some public files
</commit_message>
<xml_diff>
--- a/public/data utilisasi.xlsx
+++ b/public/data utilisasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\myapp\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68913146-0030-4A77-BD98-50A80967631F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72730845-52BF-4095-8AE9-CFEF4B52D6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{6836D58E-29B9-4D47-A867-BEE82B578EED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6836D58E-29B9-4D47-A867-BEE82B578EED}"/>
   </bookViews>
   <sheets>
     <sheet name="sumbagut" sheetId="1" r:id="rId1"/>
@@ -3471,15 +3471,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B36CC-6BF7-4A6F-A4D4-40503F5C0013}">
   <dimension ref="A2:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E60" sqref="C2:E60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4493,7 +4493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{917118A0-60AE-46CB-8B43-93934C46C9DE}">
   <dimension ref="B2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>

</xml_diff>